<commit_message>
feat: implemented component relation
</commit_message>
<xml_diff>
--- a/src/assets/angular.xlsx
+++ b/src/assets/angular.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\503300634\priya\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\503300634\priya\angular-application\dav\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC60021B-E453-4758-9FA3-67DB44F96167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{929FEBD5-0178-47B6-AE29-9C823A198907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BD6E4F09-FECA-4B89-B15A-656161B7343D}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="471">
   <si>
     <t>Services</t>
   </si>
@@ -1529,6 +1529,12 @@
   </si>
   <si>
     <t>rxjs - https://blog.bitsrc.io/mastering-rxjs-operators-unlocking-the-power-of-angular-af375e45d4eb</t>
+  </si>
+  <si>
+    <t>https://www.digitalocean.com/community/tutorials/angular-hostbinding-hostlistener</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -1975,7 +1981,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2146,6 +2152,10 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2154,6 +2164,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2163,6 +2174,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2181,24 +2194,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2277,10 +2288,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2598,8 +2605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F1ECCB1-E4F6-4BD5-A5D2-4C5E1A74C7E1}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2628,10 +2635,10 @@
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="60" t="s">
+      <c r="E2" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="61"/>
+      <c r="F2" s="63"/>
     </row>
     <row r="3" spans="1:6" ht="22.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="56" t="s">
@@ -2657,7 +2664,7 @@
       <c r="E4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="107" t="s">
+      <c r="F4" s="60" t="s">
         <v>464</v>
       </c>
     </row>
@@ -2706,10 +2713,10 @@
       </c>
       <c r="C8" s="54"/>
       <c r="D8" s="54"/>
-      <c r="E8" s="107" t="s">
+      <c r="E8" s="60" t="s">
         <v>467</v>
       </c>
-      <c r="F8" s="108" t="s">
+      <c r="F8" s="61" t="s">
         <v>466</v>
       </c>
     </row>
@@ -2785,21 +2792,25 @@
       <c r="A15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="62"/>
-      <c r="C15" s="62"/>
-      <c r="D15" s="62"/>
-      <c r="E15" s="62"/>
-      <c r="F15" s="62"/>
+      <c r="B15" s="64" t="s">
+        <v>463</v>
+      </c>
+      <c r="C15" s="64"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="66" t="s">
+        <v>469</v>
+      </c>
+      <c r="F15" s="64"/>
     </row>
     <row r="16" spans="1:6" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="63"/>
-      <c r="C16" s="63"/>
-      <c r="D16" s="63"/>
-      <c r="E16" s="63"/>
-      <c r="F16" s="63"/>
+      <c r="B16" s="65"/>
+      <c r="C16" s="65"/>
+      <c r="D16" s="65"/>
+      <c r="E16" s="65"/>
+      <c r="F16" s="65"/>
     </row>
     <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="57" t="s">
@@ -2945,71 +2956,71 @@
       <c r="A31" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="62"/>
-      <c r="C31" s="62"/>
-      <c r="D31" s="62"/>
-      <c r="E31" s="62"/>
-      <c r="F31" s="62"/>
+      <c r="B31" s="64"/>
+      <c r="C31" s="64"/>
+      <c r="D31" s="64"/>
+      <c r="E31" s="64"/>
+      <c r="F31" s="64"/>
     </row>
     <row r="32" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="53"/>
-      <c r="B32" s="63"/>
-      <c r="C32" s="63"/>
-      <c r="D32" s="63"/>
-      <c r="E32" s="63"/>
-      <c r="F32" s="63"/>
+      <c r="B32" s="65"/>
+      <c r="C32" s="65"/>
+      <c r="D32" s="65"/>
+      <c r="E32" s="65"/>
+      <c r="F32" s="65"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="62"/>
-      <c r="C33" s="62"/>
-      <c r="D33" s="62"/>
-      <c r="E33" s="62"/>
-      <c r="F33" s="62"/>
+      <c r="B33" s="64"/>
+      <c r="C33" s="64"/>
+      <c r="D33" s="64"/>
+      <c r="E33" s="64"/>
+      <c r="F33" s="64"/>
     </row>
     <row r="34" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="63"/>
-      <c r="C34" s="63"/>
-      <c r="D34" s="63"/>
-      <c r="E34" s="63"/>
-      <c r="F34" s="63"/>
+      <c r="B34" s="65"/>
+      <c r="C34" s="65"/>
+      <c r="D34" s="65"/>
+      <c r="E34" s="65"/>
+      <c r="F34" s="65"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="62"/>
-      <c r="B35" s="62"/>
-      <c r="C35" s="62"/>
-      <c r="D35" s="62"/>
-      <c r="E35" s="62"/>
-      <c r="F35" s="62"/>
+      <c r="A35" s="64"/>
+      <c r="B35" s="64"/>
+      <c r="C35" s="64"/>
+      <c r="D35" s="64"/>
+      <c r="E35" s="64"/>
+      <c r="F35" s="64"/>
     </row>
     <row r="36" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="63"/>
-      <c r="B36" s="63"/>
-      <c r="C36" s="63"/>
-      <c r="D36" s="63"/>
-      <c r="E36" s="63"/>
-      <c r="F36" s="63"/>
+      <c r="A36" s="65"/>
+      <c r="B36" s="65"/>
+      <c r="C36" s="65"/>
+      <c r="D36" s="65"/>
+      <c r="E36" s="65"/>
+      <c r="F36" s="65"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="62"/>
-      <c r="B37" s="62"/>
-      <c r="C37" s="62"/>
-      <c r="D37" s="62"/>
-      <c r="E37" s="62"/>
-      <c r="F37" s="62"/>
+      <c r="A37" s="64"/>
+      <c r="B37" s="64"/>
+      <c r="C37" s="64"/>
+      <c r="D37" s="64"/>
+      <c r="E37" s="64"/>
+      <c r="F37" s="64"/>
     </row>
     <row r="38" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="63"/>
-      <c r="B38" s="63"/>
-      <c r="C38" s="63"/>
-      <c r="D38" s="63"/>
-      <c r="E38" s="63"/>
-      <c r="F38" s="63"/>
+      <c r="A38" s="65"/>
+      <c r="B38" s="65"/>
+      <c r="C38" s="65"/>
+      <c r="D38" s="65"/>
+      <c r="E38" s="65"/>
+      <c r="F38" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="28">
@@ -3044,9 +3055,10 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F8" r:id="rId1" xr:uid="{C0A5AF24-A35B-434A-A09C-3EAEAFED6907}"/>
+    <hyperlink ref="E15" r:id="rId2" xr:uid="{1323E073-1882-4875-841B-C8BC42FB756F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -3202,10 +3214,10 @@
         <v>45</v>
       </c>
       <c r="C10" s="9"/>
-      <c r="D10" s="64" t="s">
+      <c r="D10" s="67" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="66"/>
+      <c r="E10" s="69"/>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
@@ -3232,10 +3244,10 @@
         <v>48</v>
       </c>
       <c r="C12" s="9"/>
-      <c r="D12" s="64" t="s">
+      <c r="D12" s="67" t="s">
         <v>49</v>
       </c>
-      <c r="E12" s="66"/>
+      <c r="E12" s="69"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
@@ -3248,10 +3260,10 @@
         <v>50</v>
       </c>
       <c r="C13" s="9"/>
-      <c r="D13" s="64" t="s">
+      <c r="D13" s="67" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="66"/>
+      <c r="E13" s="69"/>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
@@ -3334,12 +3346,12 @@
         <v>56</v>
       </c>
       <c r="C19" s="9"/>
-      <c r="D19" s="64" t="s">
+      <c r="D19" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="E19" s="65"/>
-      <c r="F19" s="65"/>
-      <c r="G19" s="66"/>
+      <c r="E19" s="68"/>
+      <c r="F19" s="68"/>
+      <c r="G19" s="69"/>
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
       <c r="J19" s="9"/>
@@ -3465,12 +3477,12 @@
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
-      <c r="G28" s="64" t="s">
+      <c r="G28" s="67" t="s">
         <v>67</v>
       </c>
-      <c r="H28" s="65"/>
-      <c r="I28" s="65"/>
-      <c r="J28" s="66"/>
+      <c r="H28" s="68"/>
+      <c r="I28" s="68"/>
+      <c r="J28" s="69"/>
     </row>
     <row r="29" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="12"/>
@@ -3989,13 +4001,13 @@
       <c r="D65" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="E65" s="64" t="s">
+      <c r="E65" s="67" t="s">
         <v>107</v>
       </c>
-      <c r="F65" s="65"/>
-      <c r="G65" s="65"/>
-      <c r="H65" s="65"/>
-      <c r="I65" s="66"/>
+      <c r="F65" s="68"/>
+      <c r="G65" s="68"/>
+      <c r="H65" s="68"/>
+      <c r="I65" s="69"/>
       <c r="J65" s="9"/>
     </row>
     <row r="66" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -4257,7 +4269,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15:F15"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4427,10 +4439,10 @@
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
-      <c r="E15" s="64" t="s">
+      <c r="E15" s="67" t="s">
         <v>139</v>
       </c>
-      <c r="F15" s="66"/>
+      <c r="F15" s="69"/>
       <c r="G15" s="9"/>
     </row>
     <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -4513,7 +4525,7 @@
   <dimension ref="A1:R63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4887,56 +4899,56 @@
       <c r="R15" s="17"/>
     </row>
     <row r="16" spans="1:18" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="67"/>
+      <c r="A16" s="72"/>
       <c r="B16" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="C16" s="67"/>
-      <c r="D16" s="75" t="s">
+      <c r="C16" s="72"/>
+      <c r="D16" s="78" t="s">
         <v>178</v>
       </c>
-      <c r="E16" s="67" t="s">
+      <c r="E16" s="72" t="s">
         <v>179</v>
       </c>
-      <c r="F16" s="73"/>
-      <c r="G16" s="73"/>
-      <c r="H16" s="67" t="s">
+      <c r="F16" s="70"/>
+      <c r="G16" s="70"/>
+      <c r="H16" s="72" t="s">
         <v>180</v>
       </c>
-      <c r="I16" s="60" t="s">
+      <c r="I16" s="62" t="s">
         <v>181</v>
       </c>
-      <c r="J16" s="69"/>
-      <c r="K16" s="69"/>
-      <c r="L16" s="69"/>
-      <c r="M16" s="69"/>
-      <c r="N16" s="69"/>
-      <c r="O16" s="69"/>
-      <c r="P16" s="61"/>
-      <c r="Q16" s="73"/>
-      <c r="R16" s="73"/>
+      <c r="J16" s="74"/>
+      <c r="K16" s="74"/>
+      <c r="L16" s="74"/>
+      <c r="M16" s="74"/>
+      <c r="N16" s="74"/>
+      <c r="O16" s="74"/>
+      <c r="P16" s="63"/>
+      <c r="Q16" s="70"/>
+      <c r="R16" s="70"/>
     </row>
     <row r="17" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="68"/>
+      <c r="A17" s="73"/>
       <c r="B17" s="23" t="s">
         <v>177</v>
       </c>
-      <c r="C17" s="68"/>
-      <c r="D17" s="76"/>
-      <c r="E17" s="68"/>
-      <c r="F17" s="74"/>
-      <c r="G17" s="74"/>
-      <c r="H17" s="68"/>
-      <c r="I17" s="70"/>
-      <c r="J17" s="71"/>
-      <c r="K17" s="71"/>
-      <c r="L17" s="71"/>
-      <c r="M17" s="71"/>
-      <c r="N17" s="71"/>
-      <c r="O17" s="71"/>
-      <c r="P17" s="72"/>
-      <c r="Q17" s="74"/>
-      <c r="R17" s="74"/>
+      <c r="C17" s="73"/>
+      <c r="D17" s="79"/>
+      <c r="E17" s="73"/>
+      <c r="F17" s="71"/>
+      <c r="G17" s="71"/>
+      <c r="H17" s="73"/>
+      <c r="I17" s="75"/>
+      <c r="J17" s="76"/>
+      <c r="K17" s="76"/>
+      <c r="L17" s="76"/>
+      <c r="M17" s="76"/>
+      <c r="N17" s="76"/>
+      <c r="O17" s="76"/>
+      <c r="P17" s="77"/>
+      <c r="Q17" s="71"/>
+      <c r="R17" s="71"/>
     </row>
     <row r="18" spans="1:18" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A18" s="12"/>
@@ -5073,48 +5085,48 @@
       <c r="R23" s="17"/>
     </row>
     <row r="24" spans="1:18" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="67"/>
+      <c r="A24" s="72"/>
       <c r="B24" s="22" t="s">
         <v>189</v>
       </c>
-      <c r="C24" s="67"/>
-      <c r="D24" s="73"/>
-      <c r="E24" s="73"/>
-      <c r="F24" s="73"/>
-      <c r="G24" s="73"/>
-      <c r="H24" s="73"/>
-      <c r="I24" s="73"/>
-      <c r="J24" s="73"/>
-      <c r="K24" s="73"/>
-      <c r="L24" s="73"/>
-      <c r="M24" s="73"/>
-      <c r="N24" s="73"/>
-      <c r="O24" s="73"/>
-      <c r="P24" s="73"/>
-      <c r="Q24" s="73"/>
-      <c r="R24" s="73"/>
+      <c r="C24" s="72"/>
+      <c r="D24" s="70"/>
+      <c r="E24" s="70"/>
+      <c r="F24" s="70"/>
+      <c r="G24" s="70"/>
+      <c r="H24" s="70"/>
+      <c r="I24" s="70"/>
+      <c r="J24" s="70"/>
+      <c r="K24" s="70"/>
+      <c r="L24" s="70"/>
+      <c r="M24" s="70"/>
+      <c r="N24" s="70"/>
+      <c r="O24" s="70"/>
+      <c r="P24" s="70"/>
+      <c r="Q24" s="70"/>
+      <c r="R24" s="70"/>
     </row>
     <row r="25" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="68"/>
+      <c r="A25" s="73"/>
       <c r="B25" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="C25" s="68"/>
-      <c r="D25" s="74"/>
-      <c r="E25" s="74"/>
-      <c r="F25" s="74"/>
-      <c r="G25" s="74"/>
-      <c r="H25" s="74"/>
-      <c r="I25" s="74"/>
-      <c r="J25" s="74"/>
-      <c r="K25" s="74"/>
-      <c r="L25" s="74"/>
-      <c r="M25" s="74"/>
-      <c r="N25" s="74"/>
-      <c r="O25" s="74"/>
-      <c r="P25" s="74"/>
-      <c r="Q25" s="74"/>
-      <c r="R25" s="74"/>
+      <c r="C25" s="73"/>
+      <c r="D25" s="71"/>
+      <c r="E25" s="71"/>
+      <c r="F25" s="71"/>
+      <c r="G25" s="71"/>
+      <c r="H25" s="71"/>
+      <c r="I25" s="71"/>
+      <c r="J25" s="71"/>
+      <c r="K25" s="71"/>
+      <c r="L25" s="71"/>
+      <c r="M25" s="71"/>
+      <c r="N25" s="71"/>
+      <c r="O25" s="71"/>
+      <c r="P25" s="71"/>
+      <c r="Q25" s="71"/>
+      <c r="R25" s="71"/>
     </row>
     <row r="26" spans="1:18" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A26" s="12"/>
@@ -5187,120 +5199,120 @@
       <c r="R28" s="17"/>
     </row>
     <row r="29" spans="1:18" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A29" s="67"/>
-      <c r="B29" s="77" t="s">
+      <c r="A29" s="72"/>
+      <c r="B29" s="81" t="s">
         <v>196</v>
       </c>
-      <c r="C29" s="67"/>
+      <c r="C29" s="72"/>
       <c r="D29" s="24" t="s">
         <v>197</v>
       </c>
-      <c r="E29" s="73"/>
-      <c r="F29" s="73"/>
-      <c r="G29" s="73"/>
-      <c r="H29" s="73"/>
-      <c r="I29" s="73"/>
-      <c r="J29" s="73"/>
-      <c r="K29" s="73"/>
-      <c r="L29" s="73"/>
-      <c r="M29" s="73"/>
-      <c r="N29" s="73"/>
-      <c r="O29" s="73"/>
-      <c r="P29" s="73"/>
-      <c r="Q29" s="73"/>
-      <c r="R29" s="73"/>
+      <c r="E29" s="70"/>
+      <c r="F29" s="70"/>
+      <c r="G29" s="70"/>
+      <c r="H29" s="70"/>
+      <c r="I29" s="70"/>
+      <c r="J29" s="70"/>
+      <c r="K29" s="70"/>
+      <c r="L29" s="70"/>
+      <c r="M29" s="70"/>
+      <c r="N29" s="70"/>
+      <c r="O29" s="70"/>
+      <c r="P29" s="70"/>
+      <c r="Q29" s="70"/>
+      <c r="R29" s="70"/>
     </row>
     <row r="30" spans="1:18" ht="42" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="68"/>
-      <c r="B30" s="78"/>
-      <c r="C30" s="68"/>
+      <c r="A30" s="73"/>
+      <c r="B30" s="83"/>
+      <c r="C30" s="73"/>
       <c r="D30" s="25" t="s">
         <v>198</v>
       </c>
-      <c r="E30" s="74"/>
-      <c r="F30" s="74"/>
-      <c r="G30" s="74"/>
-      <c r="H30" s="74"/>
-      <c r="I30" s="74"/>
-      <c r="J30" s="74"/>
-      <c r="K30" s="74"/>
-      <c r="L30" s="74"/>
-      <c r="M30" s="74"/>
-      <c r="N30" s="74"/>
-      <c r="O30" s="74"/>
-      <c r="P30" s="74"/>
-      <c r="Q30" s="74"/>
-      <c r="R30" s="74"/>
+      <c r="E30" s="71"/>
+      <c r="F30" s="71"/>
+      <c r="G30" s="71"/>
+      <c r="H30" s="71"/>
+      <c r="I30" s="71"/>
+      <c r="J30" s="71"/>
+      <c r="K30" s="71"/>
+      <c r="L30" s="71"/>
+      <c r="M30" s="71"/>
+      <c r="N30" s="71"/>
+      <c r="O30" s="71"/>
+      <c r="P30" s="71"/>
+      <c r="Q30" s="71"/>
+      <c r="R30" s="71"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A31" s="67"/>
-      <c r="B31" s="77" t="s">
+      <c r="A31" s="72"/>
+      <c r="B31" s="81" t="s">
         <v>199</v>
       </c>
-      <c r="C31" s="67"/>
-      <c r="D31" s="81" t="s">
+      <c r="C31" s="72"/>
+      <c r="D31" s="84" t="s">
         <v>200</v>
       </c>
       <c r="E31" s="26" t="s">
         <v>201</v>
       </c>
-      <c r="F31" s="73"/>
-      <c r="G31" s="73"/>
-      <c r="H31" s="73"/>
-      <c r="I31" s="73"/>
-      <c r="J31" s="73"/>
-      <c r="K31" s="73"/>
-      <c r="L31" s="73"/>
-      <c r="M31" s="73"/>
-      <c r="N31" s="73"/>
-      <c r="O31" s="73"/>
-      <c r="P31" s="73"/>
-      <c r="Q31" s="73"/>
-      <c r="R31" s="73"/>
+      <c r="F31" s="70"/>
+      <c r="G31" s="70"/>
+      <c r="H31" s="70"/>
+      <c r="I31" s="70"/>
+      <c r="J31" s="70"/>
+      <c r="K31" s="70"/>
+      <c r="L31" s="70"/>
+      <c r="M31" s="70"/>
+      <c r="N31" s="70"/>
+      <c r="O31" s="70"/>
+      <c r="P31" s="70"/>
+      <c r="Q31" s="70"/>
+      <c r="R31" s="70"/>
     </row>
     <row r="32" spans="1:18" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="79"/>
-      <c r="B32" s="80"/>
-      <c r="C32" s="79"/>
-      <c r="D32" s="82"/>
+      <c r="A32" s="80"/>
+      <c r="B32" s="82"/>
+      <c r="C32" s="80"/>
+      <c r="D32" s="85"/>
       <c r="E32" s="27" t="s">
         <v>202</v>
       </c>
-      <c r="F32" s="84"/>
-      <c r="G32" s="84"/>
-      <c r="H32" s="84"/>
-      <c r="I32" s="84"/>
-      <c r="J32" s="84"/>
-      <c r="K32" s="84"/>
-      <c r="L32" s="84"/>
-      <c r="M32" s="84"/>
-      <c r="N32" s="84"/>
-      <c r="O32" s="84"/>
-      <c r="P32" s="84"/>
-      <c r="Q32" s="84"/>
-      <c r="R32" s="84"/>
+      <c r="F32" s="87"/>
+      <c r="G32" s="87"/>
+      <c r="H32" s="87"/>
+      <c r="I32" s="87"/>
+      <c r="J32" s="87"/>
+      <c r="K32" s="87"/>
+      <c r="L32" s="87"/>
+      <c r="M32" s="87"/>
+      <c r="N32" s="87"/>
+      <c r="O32" s="87"/>
+      <c r="P32" s="87"/>
+      <c r="Q32" s="87"/>
+      <c r="R32" s="87"/>
     </row>
     <row r="33" spans="1:18" ht="42" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="68"/>
-      <c r="B33" s="78"/>
-      <c r="C33" s="68"/>
-      <c r="D33" s="83"/>
+      <c r="A33" s="73"/>
+      <c r="B33" s="83"/>
+      <c r="C33" s="73"/>
+      <c r="D33" s="86"/>
       <c r="E33" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="F33" s="74"/>
-      <c r="G33" s="74"/>
-      <c r="H33" s="74"/>
-      <c r="I33" s="74"/>
-      <c r="J33" s="74"/>
-      <c r="K33" s="74"/>
-      <c r="L33" s="74"/>
-      <c r="M33" s="74"/>
-      <c r="N33" s="74"/>
-      <c r="O33" s="74"/>
-      <c r="P33" s="74"/>
-      <c r="Q33" s="74"/>
-      <c r="R33" s="74"/>
+      <c r="F33" s="71"/>
+      <c r="G33" s="71"/>
+      <c r="H33" s="71"/>
+      <c r="I33" s="71"/>
+      <c r="J33" s="71"/>
+      <c r="K33" s="71"/>
+      <c r="L33" s="71"/>
+      <c r="M33" s="71"/>
+      <c r="N33" s="71"/>
+      <c r="O33" s="71"/>
+      <c r="P33" s="71"/>
+      <c r="Q33" s="71"/>
+      <c r="R33" s="71"/>
     </row>
     <row r="34" spans="1:18" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A34" s="17"/>
@@ -5400,10 +5412,10 @@
       <c r="A38" s="17"/>
       <c r="B38" s="17"/>
       <c r="C38" s="17"/>
-      <c r="D38" s="64" t="s">
+      <c r="D38" s="67" t="s">
         <v>211</v>
       </c>
-      <c r="E38" s="66"/>
+      <c r="E38" s="69"/>
       <c r="F38" s="17"/>
       <c r="G38" s="17"/>
       <c r="H38" s="17"/>
@@ -5419,50 +5431,50 @@
       <c r="R38" s="17"/>
     </row>
     <row r="39" spans="1:18" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="67"/>
+      <c r="A39" s="72"/>
       <c r="B39" s="24" t="s">
         <v>212</v>
       </c>
-      <c r="C39" s="67"/>
-      <c r="D39" s="85" t="s">
+      <c r="C39" s="72"/>
+      <c r="D39" s="88" t="s">
         <v>214</v>
       </c>
-      <c r="E39" s="86"/>
-      <c r="F39" s="73"/>
-      <c r="G39" s="73"/>
-      <c r="H39" s="73"/>
-      <c r="I39" s="73"/>
-      <c r="J39" s="73"/>
-      <c r="K39" s="73"/>
-      <c r="L39" s="73"/>
-      <c r="M39" s="73"/>
-      <c r="N39" s="73"/>
-      <c r="O39" s="73"/>
-      <c r="P39" s="73"/>
-      <c r="Q39" s="73"/>
-      <c r="R39" s="73"/>
+      <c r="E39" s="89"/>
+      <c r="F39" s="70"/>
+      <c r="G39" s="70"/>
+      <c r="H39" s="70"/>
+      <c r="I39" s="70"/>
+      <c r="J39" s="70"/>
+      <c r="K39" s="70"/>
+      <c r="L39" s="70"/>
+      <c r="M39" s="70"/>
+      <c r="N39" s="70"/>
+      <c r="O39" s="70"/>
+      <c r="P39" s="70"/>
+      <c r="Q39" s="70"/>
+      <c r="R39" s="70"/>
     </row>
     <row r="40" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="68"/>
+      <c r="A40" s="73"/>
       <c r="B40" s="25" t="s">
         <v>213</v>
       </c>
-      <c r="C40" s="68"/>
-      <c r="D40" s="87"/>
-      <c r="E40" s="88"/>
-      <c r="F40" s="74"/>
-      <c r="G40" s="74"/>
-      <c r="H40" s="74"/>
-      <c r="I40" s="74"/>
-      <c r="J40" s="74"/>
-      <c r="K40" s="74"/>
-      <c r="L40" s="74"/>
-      <c r="M40" s="74"/>
-      <c r="N40" s="74"/>
-      <c r="O40" s="74"/>
-      <c r="P40" s="74"/>
-      <c r="Q40" s="74"/>
-      <c r="R40" s="74"/>
+      <c r="C40" s="73"/>
+      <c r="D40" s="90"/>
+      <c r="E40" s="91"/>
+      <c r="F40" s="71"/>
+      <c r="G40" s="71"/>
+      <c r="H40" s="71"/>
+      <c r="I40" s="71"/>
+      <c r="J40" s="71"/>
+      <c r="K40" s="71"/>
+      <c r="L40" s="71"/>
+      <c r="M40" s="71"/>
+      <c r="N40" s="71"/>
+      <c r="O40" s="71"/>
+      <c r="P40" s="71"/>
+      <c r="Q40" s="71"/>
+      <c r="R40" s="71"/>
     </row>
     <row r="41" spans="1:18" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A41" s="17"/>
@@ -5487,96 +5499,96 @@
       <c r="R41" s="17"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A42" s="67"/>
-      <c r="B42" s="67" t="s">
+      <c r="A42" s="72"/>
+      <c r="B42" s="72" t="s">
         <v>216</v>
       </c>
-      <c r="C42" s="67"/>
-      <c r="D42" s="67" t="s">
+      <c r="C42" s="72"/>
+      <c r="D42" s="72" t="s">
         <v>215</v>
       </c>
       <c r="E42" s="26" t="s">
         <v>217</v>
       </c>
-      <c r="F42" s="73"/>
-      <c r="G42" s="73"/>
-      <c r="H42" s="73"/>
-      <c r="I42" s="73"/>
-      <c r="J42" s="73"/>
-      <c r="K42" s="73"/>
-      <c r="L42" s="73"/>
-      <c r="M42" s="73"/>
-      <c r="N42" s="73"/>
-      <c r="O42" s="73"/>
-      <c r="P42" s="73"/>
-      <c r="Q42" s="73"/>
-      <c r="R42" s="73"/>
+      <c r="F42" s="70"/>
+      <c r="G42" s="70"/>
+      <c r="H42" s="70"/>
+      <c r="I42" s="70"/>
+      <c r="J42" s="70"/>
+      <c r="K42" s="70"/>
+      <c r="L42" s="70"/>
+      <c r="M42" s="70"/>
+      <c r="N42" s="70"/>
+      <c r="O42" s="70"/>
+      <c r="P42" s="70"/>
+      <c r="Q42" s="70"/>
+      <c r="R42" s="70"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A43" s="79"/>
-      <c r="B43" s="79"/>
-      <c r="C43" s="79"/>
-      <c r="D43" s="79"/>
+      <c r="A43" s="80"/>
+      <c r="B43" s="80"/>
+      <c r="C43" s="80"/>
+      <c r="D43" s="80"/>
       <c r="E43" s="27" t="s">
         <v>218</v>
       </c>
-      <c r="F43" s="84"/>
-      <c r="G43" s="84"/>
-      <c r="H43" s="84"/>
-      <c r="I43" s="84"/>
-      <c r="J43" s="84"/>
-      <c r="K43" s="84"/>
-      <c r="L43" s="84"/>
-      <c r="M43" s="84"/>
-      <c r="N43" s="84"/>
-      <c r="O43" s="84"/>
-      <c r="P43" s="84"/>
-      <c r="Q43" s="84"/>
-      <c r="R43" s="84"/>
+      <c r="F43" s="87"/>
+      <c r="G43" s="87"/>
+      <c r="H43" s="87"/>
+      <c r="I43" s="87"/>
+      <c r="J43" s="87"/>
+      <c r="K43" s="87"/>
+      <c r="L43" s="87"/>
+      <c r="M43" s="87"/>
+      <c r="N43" s="87"/>
+      <c r="O43" s="87"/>
+      <c r="P43" s="87"/>
+      <c r="Q43" s="87"/>
+      <c r="R43" s="87"/>
     </row>
     <row r="44" spans="1:18" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A44" s="79"/>
-      <c r="B44" s="79"/>
-      <c r="C44" s="79"/>
-      <c r="D44" s="79"/>
+      <c r="A44" s="80"/>
+      <c r="B44" s="80"/>
+      <c r="C44" s="80"/>
+      <c r="D44" s="80"/>
       <c r="E44" s="29" t="s">
         <v>219</v>
       </c>
-      <c r="F44" s="84"/>
-      <c r="G44" s="84"/>
-      <c r="H44" s="84"/>
-      <c r="I44" s="84"/>
-      <c r="J44" s="84"/>
-      <c r="K44" s="84"/>
-      <c r="L44" s="84"/>
-      <c r="M44" s="84"/>
-      <c r="N44" s="84"/>
-      <c r="O44" s="84"/>
-      <c r="P44" s="84"/>
-      <c r="Q44" s="84"/>
-      <c r="R44" s="84"/>
+      <c r="F44" s="87"/>
+      <c r="G44" s="87"/>
+      <c r="H44" s="87"/>
+      <c r="I44" s="87"/>
+      <c r="J44" s="87"/>
+      <c r="K44" s="87"/>
+      <c r="L44" s="87"/>
+      <c r="M44" s="87"/>
+      <c r="N44" s="87"/>
+      <c r="O44" s="87"/>
+      <c r="P44" s="87"/>
+      <c r="Q44" s="87"/>
+      <c r="R44" s="87"/>
     </row>
     <row r="45" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="68"/>
-      <c r="B45" s="68"/>
-      <c r="C45" s="68"/>
-      <c r="D45" s="68"/>
+      <c r="A45" s="73"/>
+      <c r="B45" s="73"/>
+      <c r="C45" s="73"/>
+      <c r="D45" s="73"/>
       <c r="E45" s="25" t="s">
         <v>220</v>
       </c>
-      <c r="F45" s="74"/>
-      <c r="G45" s="74"/>
-      <c r="H45" s="74"/>
-      <c r="I45" s="74"/>
-      <c r="J45" s="74"/>
-      <c r="K45" s="74"/>
-      <c r="L45" s="74"/>
-      <c r="M45" s="74"/>
-      <c r="N45" s="74"/>
-      <c r="O45" s="74"/>
-      <c r="P45" s="74"/>
-      <c r="Q45" s="74"/>
-      <c r="R45" s="74"/>
+      <c r="F45" s="71"/>
+      <c r="G45" s="71"/>
+      <c r="H45" s="71"/>
+      <c r="I45" s="71"/>
+      <c r="J45" s="71"/>
+      <c r="K45" s="71"/>
+      <c r="L45" s="71"/>
+      <c r="M45" s="71"/>
+      <c r="N45" s="71"/>
+      <c r="O45" s="71"/>
+      <c r="P45" s="71"/>
+      <c r="Q45" s="71"/>
+      <c r="R45" s="71"/>
     </row>
     <row r="46" spans="1:18" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A46" s="12"/>
@@ -5631,54 +5643,54 @@
       <c r="R47" s="17"/>
     </row>
     <row r="48" spans="1:18" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A48" s="67"/>
-      <c r="B48" s="67" t="s">
+      <c r="A48" s="72"/>
+      <c r="B48" s="72" t="s">
         <v>227</v>
       </c>
-      <c r="C48" s="67"/>
+      <c r="C48" s="72"/>
       <c r="D48" s="24" t="s">
         <v>228</v>
       </c>
-      <c r="E48" s="89" t="s">
+      <c r="E48" s="92" t="s">
         <v>230</v>
       </c>
-      <c r="F48" s="73"/>
-      <c r="G48" s="73"/>
-      <c r="H48" s="73"/>
-      <c r="I48" s="73"/>
-      <c r="J48" s="73"/>
-      <c r="K48" s="73"/>
-      <c r="L48" s="73"/>
-      <c r="M48" s="73"/>
-      <c r="N48" s="73"/>
-      <c r="O48" s="73"/>
-      <c r="P48" s="73"/>
-      <c r="Q48" s="73"/>
-      <c r="R48" s="73"/>
+      <c r="F48" s="70"/>
+      <c r="G48" s="70"/>
+      <c r="H48" s="70"/>
+      <c r="I48" s="70"/>
+      <c r="J48" s="70"/>
+      <c r="K48" s="70"/>
+      <c r="L48" s="70"/>
+      <c r="M48" s="70"/>
+      <c r="N48" s="70"/>
+      <c r="O48" s="70"/>
+      <c r="P48" s="70"/>
+      <c r="Q48" s="70"/>
+      <c r="R48" s="70"/>
     </row>
     <row r="49" spans="1:18" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="68"/>
-      <c r="B49" s="68"/>
-      <c r="C49" s="68"/>
+      <c r="A49" s="73"/>
+      <c r="B49" s="73"/>
+      <c r="C49" s="73"/>
       <c r="D49" s="25" t="s">
         <v>229</v>
       </c>
-      <c r="E49" s="68"/>
-      <c r="F49" s="74"/>
-      <c r="G49" s="74"/>
-      <c r="H49" s="74"/>
-      <c r="I49" s="74"/>
-      <c r="J49" s="74"/>
-      <c r="K49" s="74"/>
-      <c r="L49" s="74"/>
-      <c r="M49" s="74"/>
-      <c r="N49" s="74"/>
-      <c r="O49" s="74"/>
-      <c r="P49" s="74"/>
-      <c r="Q49" s="74"/>
-      <c r="R49" s="74"/>
-    </row>
-    <row r="50" spans="1:18" ht="111" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="E49" s="73"/>
+      <c r="F49" s="71"/>
+      <c r="G49" s="71"/>
+      <c r="H49" s="71"/>
+      <c r="I49" s="71"/>
+      <c r="J49" s="71"/>
+      <c r="K49" s="71"/>
+      <c r="L49" s="71"/>
+      <c r="M49" s="71"/>
+      <c r="N49" s="71"/>
+      <c r="O49" s="71"/>
+      <c r="P49" s="71"/>
+      <c r="Q49" s="71"/>
+      <c r="R49" s="71"/>
+    </row>
+    <row r="50" spans="1:18" ht="28.2" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A50" s="12"/>
       <c r="B50" s="12" t="s">
         <v>231</v>
@@ -5748,7 +5760,7 @@
       <c r="Q52" s="17"/>
       <c r="R52" s="17"/>
     </row>
-    <row r="53" spans="1:18" ht="138.6" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:18" ht="28.2" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A53" s="17"/>
       <c r="B53" s="12" t="s">
         <v>236</v>
@@ -6061,6 +6073,11 @@
     <mergeCell ref="O29:O30"/>
     <mergeCell ref="N31:N33"/>
     <mergeCell ref="O31:O33"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
     <mergeCell ref="P29:P30"/>
     <mergeCell ref="Q29:Q30"/>
     <mergeCell ref="R29:R30"/>
@@ -6070,19 +6087,6 @@
     <mergeCell ref="J29:J30"/>
     <mergeCell ref="K29:K30"/>
     <mergeCell ref="L29:L30"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="K24:K25"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="I16:P17"/>
-    <mergeCell ref="Q16:Q17"/>
-    <mergeCell ref="R16:R17"/>
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="C24:C25"/>
     <mergeCell ref="D24:D25"/>
@@ -6095,13 +6099,21 @@
     <mergeCell ref="E16:E17"/>
     <mergeCell ref="F16:F17"/>
     <mergeCell ref="G16:G17"/>
+    <mergeCell ref="R24:R25"/>
+    <mergeCell ref="L24:L25"/>
+    <mergeCell ref="M24:M25"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="K24:K25"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="I16:P17"/>
+    <mergeCell ref="Q16:Q17"/>
+    <mergeCell ref="R16:R17"/>
     <mergeCell ref="N24:N25"/>
     <mergeCell ref="O24:O25"/>
     <mergeCell ref="P24:P25"/>
     <mergeCell ref="Q24:Q25"/>
-    <mergeCell ref="R24:R25"/>
-    <mergeCell ref="L24:L25"/>
-    <mergeCell ref="M24:M25"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D13" r:id="rId1" xr:uid="{4E3F4486-39CD-47F3-BC5C-874B3E54E7C8}"/>
@@ -6118,8 +6130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5269A5-4F6A-4733-9556-A52982FB4D93}">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33:D33"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6153,7 +6165,9 @@
       <c r="A2" s="32" t="s">
         <v>246</v>
       </c>
-      <c r="B2" s="12"/>
+      <c r="B2" s="12" t="s">
+        <v>470</v>
+      </c>
       <c r="C2" s="17"/>
       <c r="D2" s="17"/>
       <c r="E2" s="17"/>
@@ -6166,7 +6180,9 @@
       <c r="A3" s="32" t="s">
         <v>247</v>
       </c>
-      <c r="B3" s="12"/>
+      <c r="B3" s="12" t="s">
+        <v>470</v>
+      </c>
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
       <c r="E3" s="17"/>
@@ -6179,7 +6195,9 @@
       <c r="A4" s="32" t="s">
         <v>248</v>
       </c>
-      <c r="B4" s="12"/>
+      <c r="B4" s="12" t="s">
+        <v>470</v>
+      </c>
       <c r="C4" s="17"/>
       <c r="D4" s="17"/>
       <c r="E4" s="17"/>
@@ -6192,7 +6210,9 @@
       <c r="A5" s="32" t="s">
         <v>249</v>
       </c>
-      <c r="B5" s="12"/>
+      <c r="B5" s="12" t="s">
+        <v>470</v>
+      </c>
       <c r="C5" s="17"/>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
@@ -6205,7 +6225,9 @@
       <c r="A6" s="32" t="s">
         <v>250</v>
       </c>
-      <c r="B6" s="12"/>
+      <c r="B6" s="12" t="s">
+        <v>470</v>
+      </c>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
@@ -6218,7 +6240,9 @@
       <c r="A7" s="32" t="s">
         <v>251</v>
       </c>
-      <c r="B7" s="12"/>
+      <c r="B7" s="12" t="s">
+        <v>470</v>
+      </c>
       <c r="C7" s="17"/>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
@@ -6231,7 +6255,9 @@
       <c r="A8" s="32" t="s">
         <v>252</v>
       </c>
-      <c r="B8" s="17"/>
+      <c r="B8" s="17" t="s">
+        <v>470</v>
+      </c>
       <c r="C8" s="17"/>
       <c r="D8" s="17"/>
       <c r="E8" s="17"/>
@@ -6244,7 +6270,9 @@
       <c r="A9" s="32" t="s">
         <v>253</v>
       </c>
-      <c r="B9" s="12"/>
+      <c r="B9" s="12" t="s">
+        <v>470</v>
+      </c>
       <c r="C9" s="17"/>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
@@ -6257,7 +6285,9 @@
       <c r="A10" s="32" t="s">
         <v>254</v>
       </c>
-      <c r="B10" s="12"/>
+      <c r="B10" s="12" t="s">
+        <v>470</v>
+      </c>
       <c r="C10" s="12" t="s">
         <v>255</v>
       </c>
@@ -6272,7 +6302,9 @@
       <c r="A11" s="32" t="s">
         <v>256</v>
       </c>
-      <c r="B11" s="12"/>
+      <c r="B11" s="12" t="s">
+        <v>470</v>
+      </c>
       <c r="C11" s="17"/>
       <c r="D11" s="17"/>
       <c r="E11" s="17"/>
@@ -6285,7 +6317,9 @@
       <c r="A12" s="32" t="s">
         <v>257</v>
       </c>
-      <c r="B12" s="17"/>
+      <c r="B12" s="17" t="s">
+        <v>470</v>
+      </c>
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
       <c r="E12" s="17"/>
@@ -6298,7 +6332,9 @@
       <c r="A13" s="32" t="s">
         <v>258</v>
       </c>
-      <c r="B13" s="12"/>
+      <c r="B13" s="12" t="s">
+        <v>470</v>
+      </c>
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
       <c r="E13" s="17"/>
@@ -6311,7 +6347,9 @@
       <c r="A14" s="32" t="s">
         <v>259</v>
       </c>
-      <c r="B14" s="12"/>
+      <c r="B14" s="12" t="s">
+        <v>470</v>
+      </c>
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
       <c r="E14" s="17"/>
@@ -6324,7 +6362,9 @@
       <c r="A15" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="B15" s="12"/>
+      <c r="B15" s="12" t="s">
+        <v>470</v>
+      </c>
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
@@ -6337,7 +6377,9 @@
       <c r="A16" s="32" t="s">
         <v>261</v>
       </c>
-      <c r="B16" s="17"/>
+      <c r="B16" s="17" t="s">
+        <v>470</v>
+      </c>
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
       <c r="E16" s="17"/>
@@ -6350,7 +6392,9 @@
       <c r="A17" s="32" t="s">
         <v>262</v>
       </c>
-      <c r="B17" s="12"/>
+      <c r="B17" s="12" t="s">
+        <v>470</v>
+      </c>
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
       <c r="E17" s="17"/>
@@ -6363,7 +6407,9 @@
       <c r="A18" s="32" t="s">
         <v>263</v>
       </c>
-      <c r="B18" s="17"/>
+      <c r="B18" s="17" t="s">
+        <v>470</v>
+      </c>
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
@@ -6376,7 +6422,9 @@
       <c r="A19" s="32" t="s">
         <v>264</v>
       </c>
-      <c r="B19" s="12"/>
+      <c r="B19" s="12" t="s">
+        <v>470</v>
+      </c>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
       <c r="E19" s="17"/>
@@ -6389,7 +6437,9 @@
       <c r="A20" s="32" t="s">
         <v>265</v>
       </c>
-      <c r="B20" s="12"/>
+      <c r="B20" s="12" t="s">
+        <v>470</v>
+      </c>
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
       <c r="E20" s="17"/>
@@ -6402,7 +6452,9 @@
       <c r="A21" s="32" t="s">
         <v>266</v>
       </c>
-      <c r="B21" s="12"/>
+      <c r="B21" s="12" t="s">
+        <v>470</v>
+      </c>
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
       <c r="E21" s="17"/>
@@ -6415,7 +6467,9 @@
       <c r="A22" s="32" t="s">
         <v>267</v>
       </c>
-      <c r="B22" s="12"/>
+      <c r="B22" s="12" t="s">
+        <v>470</v>
+      </c>
       <c r="C22" s="17"/>
       <c r="D22" s="17"/>
       <c r="E22" s="17"/>
@@ -6428,7 +6482,9 @@
       <c r="A23" s="32" t="s">
         <v>268</v>
       </c>
-      <c r="B23" s="12"/>
+      <c r="B23" s="12" t="s">
+        <v>470</v>
+      </c>
       <c r="C23" s="17"/>
       <c r="D23" s="17"/>
       <c r="E23" s="17"/>
@@ -6441,7 +6497,9 @@
       <c r="A24" s="32" t="s">
         <v>269</v>
       </c>
-      <c r="B24" s="12"/>
+      <c r="B24" s="12" t="s">
+        <v>470</v>
+      </c>
       <c r="C24" s="17"/>
       <c r="D24" s="17"/>
       <c r="E24" s="17"/>
@@ -6454,7 +6512,9 @@
       <c r="A25" s="32" t="s">
         <v>270</v>
       </c>
-      <c r="B25" s="12"/>
+      <c r="B25" s="12" t="s">
+        <v>470</v>
+      </c>
       <c r="C25" s="17"/>
       <c r="D25" s="17"/>
       <c r="E25" s="17"/>
@@ -6467,7 +6527,9 @@
       <c r="A26" s="32" t="s">
         <v>271</v>
       </c>
-      <c r="B26" s="12"/>
+      <c r="B26" s="12" t="s">
+        <v>470</v>
+      </c>
       <c r="C26" s="17"/>
       <c r="D26" s="17"/>
       <c r="E26" s="17"/>
@@ -6480,7 +6542,9 @@
       <c r="A27" s="32" t="s">
         <v>272</v>
       </c>
-      <c r="B27" s="17"/>
+      <c r="B27" s="17" t="s">
+        <v>470</v>
+      </c>
       <c r="C27" s="17"/>
       <c r="D27" s="17"/>
       <c r="E27" s="17"/>
@@ -6493,7 +6557,9 @@
       <c r="A28" s="32" t="s">
         <v>273</v>
       </c>
-      <c r="B28" s="12"/>
+      <c r="B28" s="12" t="s">
+        <v>470</v>
+      </c>
       <c r="C28" s="17"/>
       <c r="D28" s="17"/>
       <c r="E28" s="17"/>
@@ -6506,7 +6572,9 @@
       <c r="A29" s="32" t="s">
         <v>274</v>
       </c>
-      <c r="B29" s="17"/>
+      <c r="B29" s="17" t="s">
+        <v>470</v>
+      </c>
       <c r="C29" s="17"/>
       <c r="D29" s="17"/>
       <c r="E29" s="17"/>
@@ -6519,7 +6587,9 @@
       <c r="A30" s="32" t="s">
         <v>275</v>
       </c>
-      <c r="B30" s="12"/>
+      <c r="B30" s="12" t="s">
+        <v>470</v>
+      </c>
       <c r="C30" s="17"/>
       <c r="D30" s="17"/>
       <c r="E30" s="17"/>
@@ -6532,7 +6602,9 @@
       <c r="A31" s="32" t="s">
         <v>276</v>
       </c>
-      <c r="B31" s="12"/>
+      <c r="B31" s="12" t="s">
+        <v>470</v>
+      </c>
       <c r="C31" s="17"/>
       <c r="D31" s="17"/>
       <c r="E31" s="17"/>
@@ -6557,10 +6629,10 @@
         <v>277</v>
       </c>
       <c r="B33" s="12"/>
-      <c r="C33" s="90" t="s">
+      <c r="C33" s="93" t="s">
         <v>278</v>
       </c>
-      <c r="D33" s="91"/>
+      <c r="D33" s="94"/>
       <c r="E33" s="17"/>
       <c r="F33" s="17"/>
       <c r="G33" s="17"/>
@@ -6654,32 +6726,32 @@
       <c r="I1" s="17"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="92" t="s">
+      <c r="A2" s="95" t="s">
         <v>281</v>
       </c>
       <c r="B2" s="35" t="s">
         <v>282</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
     </row>
     <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="93"/>
+      <c r="A3" s="96"/>
       <c r="B3" s="36" t="s">
         <v>283</v>
       </c>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
-      <c r="H3" s="74"/>
-      <c r="I3" s="74"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="71"/>
     </row>
     <row r="4" spans="1:9" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A4" s="37" t="s">
@@ -6991,13 +7063,13 @@
       <c r="B25" s="45" t="s">
         <v>320</v>
       </c>
-      <c r="C25" s="73"/>
-      <c r="D25" s="73"/>
-      <c r="E25" s="73"/>
-      <c r="F25" s="73"/>
-      <c r="G25" s="73"/>
-      <c r="H25" s="73"/>
-      <c r="I25" s="73"/>
+      <c r="C25" s="70"/>
+      <c r="D25" s="70"/>
+      <c r="E25" s="70"/>
+      <c r="F25" s="70"/>
+      <c r="G25" s="70"/>
+      <c r="H25" s="70"/>
+      <c r="I25" s="70"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="43" t="s">
@@ -7006,54 +7078,54 @@
       <c r="B26" s="45" t="s">
         <v>321</v>
       </c>
-      <c r="C26" s="84"/>
-      <c r="D26" s="84"/>
-      <c r="E26" s="84"/>
-      <c r="F26" s="84"/>
-      <c r="G26" s="84"/>
-      <c r="H26" s="84"/>
-      <c r="I26" s="84"/>
+      <c r="C26" s="87"/>
+      <c r="D26" s="87"/>
+      <c r="E26" s="87"/>
+      <c r="F26" s="87"/>
+      <c r="G26" s="87"/>
+      <c r="H26" s="87"/>
+      <c r="I26" s="87"/>
     </row>
     <row r="27" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="44" t="s">
         <v>319</v>
       </c>
       <c r="B27" s="46"/>
-      <c r="C27" s="74"/>
-      <c r="D27" s="74"/>
-      <c r="E27" s="74"/>
-      <c r="F27" s="74"/>
-      <c r="G27" s="74"/>
-      <c r="H27" s="74"/>
-      <c r="I27" s="74"/>
+      <c r="C27" s="71"/>
+      <c r="D27" s="71"/>
+      <c r="E27" s="71"/>
+      <c r="F27" s="71"/>
+      <c r="G27" s="71"/>
+      <c r="H27" s="71"/>
+      <c r="I27" s="71"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="43" t="s">
         <v>322</v>
       </c>
-      <c r="B28" s="96" t="s">
+      <c r="B28" s="99" t="s">
         <v>324</v>
       </c>
-      <c r="C28" s="73"/>
-      <c r="D28" s="73"/>
-      <c r="E28" s="73"/>
-      <c r="F28" s="73"/>
-      <c r="G28" s="73"/>
-      <c r="H28" s="73"/>
-      <c r="I28" s="73"/>
+      <c r="C28" s="70"/>
+      <c r="D28" s="70"/>
+      <c r="E28" s="70"/>
+      <c r="F28" s="70"/>
+      <c r="G28" s="70"/>
+      <c r="H28" s="70"/>
+      <c r="I28" s="70"/>
     </row>
     <row r="29" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="44" t="s">
         <v>323</v>
       </c>
-      <c r="B29" s="97"/>
-      <c r="C29" s="74"/>
-      <c r="D29" s="74"/>
-      <c r="E29" s="74"/>
-      <c r="F29" s="74"/>
-      <c r="G29" s="74"/>
-      <c r="H29" s="74"/>
-      <c r="I29" s="74"/>
+      <c r="B29" s="100"/>
+      <c r="C29" s="71"/>
+      <c r="D29" s="71"/>
+      <c r="E29" s="71"/>
+      <c r="F29" s="71"/>
+      <c r="G29" s="71"/>
+      <c r="H29" s="71"/>
+      <c r="I29" s="71"/>
     </row>
     <row r="30" spans="1:9" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A30" s="41" t="s">
@@ -7142,32 +7214,32 @@
       <c r="I35" s="17"/>
     </row>
     <row r="36" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="94" t="s">
+      <c r="A36" s="97" t="s">
         <v>335</v>
       </c>
       <c r="B36" s="45" t="s">
         <v>336</v>
       </c>
-      <c r="C36" s="73"/>
-      <c r="D36" s="73"/>
-      <c r="E36" s="73"/>
-      <c r="F36" s="73"/>
-      <c r="G36" s="73"/>
-      <c r="H36" s="73"/>
-      <c r="I36" s="73"/>
+      <c r="C36" s="70"/>
+      <c r="D36" s="70"/>
+      <c r="E36" s="70"/>
+      <c r="F36" s="70"/>
+      <c r="G36" s="70"/>
+      <c r="H36" s="70"/>
+      <c r="I36" s="70"/>
     </row>
     <row r="37" spans="1:9" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="95"/>
+      <c r="A37" s="98"/>
       <c r="B37" s="47" t="s">
         <v>337</v>
       </c>
-      <c r="C37" s="74"/>
-      <c r="D37" s="74"/>
-      <c r="E37" s="74"/>
-      <c r="F37" s="74"/>
-      <c r="G37" s="74"/>
-      <c r="H37" s="74"/>
-      <c r="I37" s="74"/>
+      <c r="C37" s="71"/>
+      <c r="D37" s="71"/>
+      <c r="E37" s="71"/>
+      <c r="F37" s="71"/>
+      <c r="G37" s="71"/>
+      <c r="H37" s="71"/>
+      <c r="I37" s="71"/>
     </row>
     <row r="38" spans="1:9" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A38" s="41" t="s">
@@ -7420,29 +7492,29 @@
       <c r="A55" s="43" t="s">
         <v>367</v>
       </c>
-      <c r="B55" s="96" t="s">
+      <c r="B55" s="99" t="s">
         <v>369</v>
       </c>
-      <c r="C55" s="73"/>
-      <c r="D55" s="73"/>
-      <c r="E55" s="73"/>
-      <c r="F55" s="73"/>
-      <c r="G55" s="73"/>
-      <c r="H55" s="73"/>
-      <c r="I55" s="73"/>
+      <c r="C55" s="70"/>
+      <c r="D55" s="70"/>
+      <c r="E55" s="70"/>
+      <c r="F55" s="70"/>
+      <c r="G55" s="70"/>
+      <c r="H55" s="70"/>
+      <c r="I55" s="70"/>
     </row>
     <row r="56" spans="1:9" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="44" t="s">
         <v>368</v>
       </c>
-      <c r="B56" s="97"/>
-      <c r="C56" s="74"/>
-      <c r="D56" s="74"/>
-      <c r="E56" s="74"/>
-      <c r="F56" s="74"/>
-      <c r="G56" s="74"/>
-      <c r="H56" s="74"/>
-      <c r="I56" s="74"/>
+      <c r="B56" s="100"/>
+      <c r="C56" s="71"/>
+      <c r="D56" s="71"/>
+      <c r="E56" s="71"/>
+      <c r="F56" s="71"/>
+      <c r="G56" s="71"/>
+      <c r="H56" s="71"/>
+      <c r="I56" s="71"/>
     </row>
     <row r="57" spans="1:9" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A57" s="41" t="s">
@@ -7538,29 +7610,29 @@
       <c r="A63" s="43" t="s">
         <v>380</v>
       </c>
-      <c r="B63" s="96" t="s">
+      <c r="B63" s="99" t="s">
         <v>382</v>
       </c>
-      <c r="C63" s="73"/>
-      <c r="D63" s="73"/>
-      <c r="E63" s="73"/>
-      <c r="F63" s="73"/>
-      <c r="G63" s="73"/>
-      <c r="H63" s="73"/>
-      <c r="I63" s="73"/>
+      <c r="C63" s="70"/>
+      <c r="D63" s="70"/>
+      <c r="E63" s="70"/>
+      <c r="F63" s="70"/>
+      <c r="G63" s="70"/>
+      <c r="H63" s="70"/>
+      <c r="I63" s="70"/>
     </row>
     <row r="64" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="44" t="s">
         <v>381</v>
       </c>
-      <c r="B64" s="97"/>
-      <c r="C64" s="74"/>
-      <c r="D64" s="74"/>
-      <c r="E64" s="74"/>
-      <c r="F64" s="74"/>
-      <c r="G64" s="74"/>
-      <c r="H64" s="74"/>
-      <c r="I64" s="74"/>
+      <c r="B64" s="100"/>
+      <c r="C64" s="71"/>
+      <c r="D64" s="71"/>
+      <c r="E64" s="71"/>
+      <c r="F64" s="71"/>
+      <c r="G64" s="71"/>
+      <c r="H64" s="71"/>
+      <c r="I64" s="71"/>
     </row>
     <row r="65" spans="1:9" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A65" s="41" t="s">
@@ -7652,113 +7724,113 @@
       <c r="A71" s="48" t="s">
         <v>390</v>
       </c>
-      <c r="B71" s="98" t="s">
+      <c r="B71" s="101" t="s">
         <v>392</v>
       </c>
-      <c r="C71" s="73"/>
-      <c r="D71" s="73"/>
-      <c r="E71" s="73"/>
-      <c r="F71" s="73"/>
-      <c r="G71" s="73"/>
-      <c r="H71" s="73"/>
-      <c r="I71" s="73"/>
+      <c r="C71" s="70"/>
+      <c r="D71" s="70"/>
+      <c r="E71" s="70"/>
+      <c r="F71" s="70"/>
+      <c r="G71" s="70"/>
+      <c r="H71" s="70"/>
+      <c r="I71" s="70"/>
     </row>
     <row r="72" spans="1:9" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="49" t="s">
         <v>391</v>
       </c>
-      <c r="B72" s="99"/>
-      <c r="C72" s="74"/>
-      <c r="D72" s="74"/>
-      <c r="E72" s="74"/>
-      <c r="F72" s="74"/>
-      <c r="G72" s="74"/>
-      <c r="H72" s="74"/>
-      <c r="I72" s="74"/>
+      <c r="B72" s="102"/>
+      <c r="C72" s="71"/>
+      <c r="D72" s="71"/>
+      <c r="E72" s="71"/>
+      <c r="F72" s="71"/>
+      <c r="G72" s="71"/>
+      <c r="H72" s="71"/>
+      <c r="I72" s="71"/>
     </row>
     <row r="73" spans="1:9" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A73" s="48" t="s">
         <v>393</v>
       </c>
-      <c r="B73" s="98" t="s">
+      <c r="B73" s="101" t="s">
         <v>395</v>
       </c>
-      <c r="C73" s="73"/>
-      <c r="D73" s="73"/>
-      <c r="E73" s="73"/>
-      <c r="F73" s="73"/>
-      <c r="G73" s="73"/>
-      <c r="H73" s="73"/>
-      <c r="I73" s="73"/>
+      <c r="C73" s="70"/>
+      <c r="D73" s="70"/>
+      <c r="E73" s="70"/>
+      <c r="F73" s="70"/>
+      <c r="G73" s="70"/>
+      <c r="H73" s="70"/>
+      <c r="I73" s="70"/>
     </row>
     <row r="74" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="49" t="s">
         <v>394</v>
       </c>
-      <c r="B74" s="99"/>
-      <c r="C74" s="74"/>
-      <c r="D74" s="74"/>
-      <c r="E74" s="74"/>
-      <c r="F74" s="74"/>
-      <c r="G74" s="74"/>
-      <c r="H74" s="74"/>
-      <c r="I74" s="74"/>
+      <c r="B74" s="102"/>
+      <c r="C74" s="71"/>
+      <c r="D74" s="71"/>
+      <c r="E74" s="71"/>
+      <c r="F74" s="71"/>
+      <c r="G74" s="71"/>
+      <c r="H74" s="71"/>
+      <c r="I74" s="71"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" s="48" t="s">
         <v>396</v>
       </c>
-      <c r="B75" s="98" t="s">
+      <c r="B75" s="101" t="s">
         <v>398</v>
       </c>
-      <c r="C75" s="73"/>
-      <c r="D75" s="73"/>
-      <c r="E75" s="73"/>
-      <c r="F75" s="73"/>
-      <c r="G75" s="73"/>
-      <c r="H75" s="73"/>
-      <c r="I75" s="73"/>
+      <c r="C75" s="70"/>
+      <c r="D75" s="70"/>
+      <c r="E75" s="70"/>
+      <c r="F75" s="70"/>
+      <c r="G75" s="70"/>
+      <c r="H75" s="70"/>
+      <c r="I75" s="70"/>
     </row>
     <row r="76" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="49" t="s">
         <v>397</v>
       </c>
-      <c r="B76" s="99"/>
-      <c r="C76" s="74"/>
-      <c r="D76" s="74"/>
-      <c r="E76" s="74"/>
-      <c r="F76" s="74"/>
-      <c r="G76" s="74"/>
-      <c r="H76" s="74"/>
-      <c r="I76" s="74"/>
+      <c r="B76" s="102"/>
+      <c r="C76" s="71"/>
+      <c r="D76" s="71"/>
+      <c r="E76" s="71"/>
+      <c r="F76" s="71"/>
+      <c r="G76" s="71"/>
+      <c r="H76" s="71"/>
+      <c r="I76" s="71"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="48" t="s">
         <v>399</v>
       </c>
-      <c r="B77" s="98" t="s">
+      <c r="B77" s="101" t="s">
         <v>401</v>
       </c>
-      <c r="C77" s="73"/>
-      <c r="D77" s="73"/>
-      <c r="E77" s="73"/>
-      <c r="F77" s="73"/>
-      <c r="G77" s="73"/>
-      <c r="H77" s="73"/>
-      <c r="I77" s="73"/>
+      <c r="C77" s="70"/>
+      <c r="D77" s="70"/>
+      <c r="E77" s="70"/>
+      <c r="F77" s="70"/>
+      <c r="G77" s="70"/>
+      <c r="H77" s="70"/>
+      <c r="I77" s="70"/>
     </row>
     <row r="78" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="49" t="s">
         <v>400</v>
       </c>
-      <c r="B78" s="100"/>
-      <c r="C78" s="74"/>
-      <c r="D78" s="74"/>
-      <c r="E78" s="74"/>
-      <c r="F78" s="74"/>
-      <c r="G78" s="74"/>
-      <c r="H78" s="74"/>
-      <c r="I78" s="74"/>
+      <c r="B78" s="103"/>
+      <c r="C78" s="71"/>
+      <c r="D78" s="71"/>
+      <c r="E78" s="71"/>
+      <c r="F78" s="71"/>
+      <c r="G78" s="71"/>
+      <c r="H78" s="71"/>
+      <c r="I78" s="71"/>
     </row>
     <row r="79" spans="1:9" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A79" s="17"/>
@@ -7799,180 +7871,180 @@
       <c r="I80" s="17"/>
     </row>
     <row r="81" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A81" s="101" t="s">
+      <c r="A81" s="104" t="s">
         <v>410</v>
       </c>
       <c r="B81" s="45" t="s">
         <v>411</v>
       </c>
-      <c r="C81" s="94" t="s">
+      <c r="C81" s="97" t="s">
         <v>413</v>
       </c>
-      <c r="D81" s="94" t="s">
+      <c r="D81" s="97" t="s">
         <v>414</v>
       </c>
-      <c r="E81" s="94" t="s">
+      <c r="E81" s="97" t="s">
         <v>415</v>
       </c>
-      <c r="F81" s="96" t="s">
+      <c r="F81" s="99" t="s">
         <v>416</v>
       </c>
-      <c r="G81" s="81" t="s">
+      <c r="G81" s="84" t="s">
         <v>417</v>
       </c>
-      <c r="H81" s="79" t="s">
+      <c r="H81" s="80" t="s">
         <v>418</v>
       </c>
-      <c r="I81" s="73"/>
+      <c r="I81" s="70"/>
     </row>
     <row r="82" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="102"/>
+      <c r="A82" s="105"/>
       <c r="B82" s="47" t="s">
         <v>412</v>
       </c>
-      <c r="C82" s="95"/>
-      <c r="D82" s="95"/>
-      <c r="E82" s="95"/>
-      <c r="F82" s="97"/>
-      <c r="G82" s="83"/>
-      <c r="H82" s="79"/>
-      <c r="I82" s="74"/>
+      <c r="C82" s="98"/>
+      <c r="D82" s="98"/>
+      <c r="E82" s="98"/>
+      <c r="F82" s="100"/>
+      <c r="G82" s="86"/>
+      <c r="H82" s="80"/>
+      <c r="I82" s="71"/>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A83" s="101" t="s">
+      <c r="A83" s="104" t="s">
         <v>419</v>
       </c>
-      <c r="B83" s="94" t="s">
+      <c r="B83" s="97" t="s">
         <v>420</v>
       </c>
       <c r="C83" s="45" t="s">
         <v>421</v>
       </c>
-      <c r="D83" s="94"/>
+      <c r="D83" s="97"/>
       <c r="E83" s="45" t="s">
         <v>423</v>
       </c>
-      <c r="F83" s="103" t="s">
+      <c r="F83" s="106" t="s">
         <v>425</v>
       </c>
-      <c r="G83" s="67" t="s">
+      <c r="G83" s="72" t="s">
         <v>426</v>
       </c>
-      <c r="H83" s="82" t="s">
+      <c r="H83" s="85" t="s">
         <v>427</v>
       </c>
-      <c r="I83" s="73"/>
+      <c r="I83" s="70"/>
     </row>
     <row r="84" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="102"/>
-      <c r="B84" s="95"/>
+      <c r="A84" s="105"/>
+      <c r="B84" s="98"/>
       <c r="C84" s="47" t="s">
         <v>422</v>
       </c>
-      <c r="D84" s="95"/>
+      <c r="D84" s="98"/>
       <c r="E84" s="47" t="s">
         <v>424</v>
       </c>
-      <c r="F84" s="104"/>
-      <c r="G84" s="68"/>
-      <c r="H84" s="83"/>
-      <c r="I84" s="74"/>
+      <c r="F84" s="107"/>
+      <c r="G84" s="73"/>
+      <c r="H84" s="86"/>
+      <c r="I84" s="71"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A85" s="94"/>
+      <c r="A85" s="97"/>
       <c r="B85" s="45" t="s">
         <v>428</v>
       </c>
       <c r="C85" s="45" t="s">
         <v>430</v>
       </c>
-      <c r="D85" s="94"/>
-      <c r="E85" s="94" t="s">
+      <c r="D85" s="97"/>
+      <c r="E85" s="97" t="s">
         <v>432</v>
       </c>
-      <c r="F85" s="96"/>
-      <c r="G85" s="67" t="s">
+      <c r="F85" s="99"/>
+      <c r="G85" s="72" t="s">
         <v>433</v>
       </c>
-      <c r="H85" s="67" t="s">
+      <c r="H85" s="72" t="s">
         <v>434</v>
       </c>
-      <c r="I85" s="73"/>
+      <c r="I85" s="70"/>
     </row>
     <row r="86" spans="1:9" ht="42" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A86" s="95"/>
+      <c r="A86" s="98"/>
       <c r="B86" s="47" t="s">
         <v>429</v>
       </c>
       <c r="C86" s="47" t="s">
         <v>431</v>
       </c>
-      <c r="D86" s="95"/>
-      <c r="E86" s="95"/>
-      <c r="F86" s="97"/>
-      <c r="G86" s="68"/>
-      <c r="H86" s="68"/>
-      <c r="I86" s="74"/>
+      <c r="D86" s="98"/>
+      <c r="E86" s="98"/>
+      <c r="F86" s="100"/>
+      <c r="G86" s="73"/>
+      <c r="H86" s="73"/>
+      <c r="I86" s="71"/>
     </row>
     <row r="87" spans="1:9" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A87" s="94"/>
-      <c r="B87" s="94"/>
-      <c r="C87" s="94" t="s">
+      <c r="A87" s="97"/>
+      <c r="B87" s="97"/>
+      <c r="C87" s="97" t="s">
         <v>435</v>
       </c>
-      <c r="D87" s="94"/>
-      <c r="E87" s="94" t="s">
+      <c r="D87" s="97"/>
+      <c r="E87" s="97" t="s">
         <v>436</v>
       </c>
-      <c r="F87" s="96"/>
-      <c r="G87" s="67" t="s">
+      <c r="F87" s="99"/>
+      <c r="G87" s="72" t="s">
         <v>437</v>
       </c>
       <c r="H87" s="24" t="s">
         <v>438</v>
       </c>
-      <c r="I87" s="73"/>
+      <c r="I87" s="70"/>
     </row>
     <row r="88" spans="1:9" ht="42" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="105"/>
-      <c r="B88" s="105"/>
-      <c r="C88" s="105"/>
-      <c r="D88" s="105"/>
-      <c r="E88" s="105"/>
-      <c r="F88" s="106"/>
-      <c r="G88" s="68"/>
+      <c r="A88" s="108"/>
+      <c r="B88" s="108"/>
+      <c r="C88" s="108"/>
+      <c r="D88" s="108"/>
+      <c r="E88" s="108"/>
+      <c r="F88" s="109"/>
+      <c r="G88" s="73"/>
       <c r="H88" s="25" t="s">
         <v>439</v>
       </c>
-      <c r="I88" s="74"/>
+      <c r="I88" s="71"/>
     </row>
     <row r="89" spans="1:9" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A89" s="73"/>
-      <c r="B89" s="73"/>
-      <c r="C89" s="73"/>
-      <c r="D89" s="73"/>
-      <c r="E89" s="73"/>
-      <c r="F89" s="73"/>
+      <c r="A89" s="70"/>
+      <c r="B89" s="70"/>
+      <c r="C89" s="70"/>
+      <c r="D89" s="70"/>
+      <c r="E89" s="70"/>
+      <c r="F89" s="70"/>
       <c r="G89" s="24" t="s">
         <v>440</v>
       </c>
-      <c r="H89" s="60" t="s">
+      <c r="H89" s="62" t="s">
         <v>442</v>
       </c>
-      <c r="I89" s="61"/>
+      <c r="I89" s="63"/>
     </row>
     <row r="90" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A90" s="74"/>
-      <c r="B90" s="74"/>
-      <c r="C90" s="74"/>
-      <c r="D90" s="74"/>
-      <c r="E90" s="74"/>
-      <c r="F90" s="74"/>
+      <c r="A90" s="71"/>
+      <c r="B90" s="71"/>
+      <c r="C90" s="71"/>
+      <c r="D90" s="71"/>
+      <c r="E90" s="71"/>
+      <c r="F90" s="71"/>
       <c r="G90" s="25" t="s">
         <v>441</v>
       </c>
-      <c r="H90" s="70"/>
-      <c r="I90" s="72"/>
+      <c r="H90" s="75"/>
+      <c r="I90" s="77"/>
     </row>
     <row r="91" spans="1:9" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A91" s="17"/>
@@ -8064,29 +8136,29 @@
       <c r="A97" s="43" t="s">
         <v>453</v>
       </c>
-      <c r="B97" s="96" t="s">
+      <c r="B97" s="99" t="s">
         <v>455</v>
       </c>
-      <c r="C97" s="73"/>
-      <c r="D97" s="73"/>
-      <c r="E97" s="73"/>
-      <c r="F97" s="73"/>
-      <c r="G97" s="73"/>
-      <c r="H97" s="73"/>
-      <c r="I97" s="73"/>
+      <c r="C97" s="70"/>
+      <c r="D97" s="70"/>
+      <c r="E97" s="70"/>
+      <c r="F97" s="70"/>
+      <c r="G97" s="70"/>
+      <c r="H97" s="70"/>
+      <c r="I97" s="70"/>
     </row>
     <row r="98" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A98" s="44" t="s">
         <v>454</v>
       </c>
-      <c r="B98" s="97"/>
-      <c r="C98" s="74"/>
-      <c r="D98" s="74"/>
-      <c r="E98" s="74"/>
-      <c r="F98" s="74"/>
-      <c r="G98" s="74"/>
-      <c r="H98" s="74"/>
-      <c r="I98" s="74"/>
+      <c r="B98" s="100"/>
+      <c r="C98" s="71"/>
+      <c r="D98" s="71"/>
+      <c r="E98" s="71"/>
+      <c r="F98" s="71"/>
+      <c r="G98" s="71"/>
+      <c r="H98" s="71"/>
+      <c r="I98" s="71"/>
     </row>
     <row r="99" spans="1:9" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A99" s="41" t="s">
@@ -8167,6 +8239,7 @@
     <mergeCell ref="D89:D90"/>
     <mergeCell ref="E89:E90"/>
     <mergeCell ref="F89:F90"/>
+    <mergeCell ref="H89:I90"/>
     <mergeCell ref="I85:I86"/>
     <mergeCell ref="A87:A88"/>
     <mergeCell ref="B87:B88"/>
@@ -8182,7 +8255,6 @@
     <mergeCell ref="F85:F86"/>
     <mergeCell ref="G85:G86"/>
     <mergeCell ref="H85:H86"/>
-    <mergeCell ref="H89:I90"/>
     <mergeCell ref="H81:H82"/>
     <mergeCell ref="I81:I82"/>
     <mergeCell ref="A83:A84"/>

</xml_diff>